<commit_message>
now its move to right name
</commit_message>
<xml_diff>
--- a/uploads/updated_gift_list.xlsx
+++ b/uploads/updated_gift_list.xlsx
@@ -543,7 +543,11 @@
           <t>adar</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -569,7 +573,11 @@
           <t>afriyat</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">

</xml_diff>

<commit_message>
lsat changes have to check mobile
</commit_message>
<xml_diff>
--- a/uploads/updated_gift_list.xlsx
+++ b/uploads/updated_gift_list.xlsx
@@ -517,7 +517,11 @@
           <t>abudi</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -543,11 +547,7 @@
           <t>adar</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -573,11 +573,7 @@
           <t>afriyat</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1188,7 +1184,11 @@
           <t>dahan</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr"/>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1357,7 +1357,11 @@
           <t>dror</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr"/>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3857,7 +3861,11 @@
           <t>sinvani</t>
         </is>
       </c>
-      <c r="C262" t="inlineStr"/>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">

</xml_diff>

<commit_message>
change background color try fix search prob
</commit_message>
<xml_diff>
--- a/uploads/updated_gift_list.xlsx
+++ b/uploads/updated_gift_list.xlsx
@@ -461,7 +461,11 @@
           <t>verifone</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -812,11 +816,7 @@
           <t>bachar</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -855,7 +855,11 @@
           <t>band</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -985,7 +989,11 @@
           <t>biton</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr"/>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1180,7 +1188,11 @@
           <t>dahan</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr"/>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1284,7 +1296,11 @@
           <t>de levi</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr"/>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1336,11 +1352,7 @@
           <t>donskoy</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">

</xml_diff>

<commit_message>
first automate search fixed
</commit_message>
<xml_diff>
--- a/uploads/updated_gift_list.xlsx
+++ b/uploads/updated_gift_list.xlsx
@@ -461,11 +461,7 @@
           <t>verifone</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -556,11 +552,7 @@
           <t>yarin</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -859,11 +851,7 @@
           <t>gabriel</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -915,7 +903,11 @@
           <t>liron</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr"/>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">

</xml_diff>

<commit_message>
new button the you can enter name you take presnet to other friend
</commit_message>
<xml_diff>
--- a/uploads/updated_gift_list.xlsx
+++ b/uploads/updated_gift_list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C290"/>
+  <dimension ref="A1:D291"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,11 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Taken By</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Received</t>
         </is>
       </c>
@@ -453,192 +458,218 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>aarar</t>
+          <t>verifone</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>moataz</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>verifone</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>יוסי</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>abdush</t>
+          <t>aarar</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>shiran</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
+          <t>moataz</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">eldad </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>abu shamala</t>
+          <t>abdush</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>zahiya</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
+          <t>shiran</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ronen</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>abudi</t>
+          <t>abu shamala</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>yossi</t>
+          <t>zahiya</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>adani</t>
+          <t>abudi</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>inbal</t>
+          <t>yossi</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>adar</t>
+          <t>adani</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>yakov</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>inbal</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>adi</t>
+          <t>adar</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>yarin</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>yakov</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>afriyat</t>
+          <t>adi</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>yaffa</t>
+          <t>yarin</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>agron</t>
+          <t>afriyat</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>yuval</t>
+          <t>yaffa</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>aharoni</t>
+          <t>agron</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>shai</t>
+          <t>yuval</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ahlofi</t>
+          <t>aharoni</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>yafit</t>
+          <t>shai</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>aladin</t>
+          <t>ahlofi</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>bahaa</t>
+          <t>yafit</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>alaluf</t>
+          <t>aladin</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>daniel</t>
+          <t>bahaa</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>almagor</t>
+          <t>alaluf</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>smadar</t>
+          <t>daniel</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -648,467 +679,473 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>mor</t>
+          <t>smadar</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>amiri</t>
+          <t>almagor</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>nerya</t>
+          <t>mor</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>arar</t>
+          <t>amiri</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>talal</t>
+          <t>nerya</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ariel</t>
+          <t>arar</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>hila</t>
+          <t>talal</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>arieli</t>
+          <t>ariel</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>niv</t>
+          <t>hila</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>arter</t>
+          <t>arieli</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>gil</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>niv</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>asulin</t>
+          <t>arter</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>achinoam</t>
+          <t>gil</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>atari</t>
+          <t>asulin</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>shely</t>
+          <t>achinoam</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>avni</t>
+          <t>atari</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>irit</t>
+          <t>shely</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>avraham moshe</t>
+          <t>avni</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>dolev</t>
+          <t>irit</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>avramzon</t>
+          <t>avraham moshe</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>amir</t>
+          <t>dolev</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>babikov</t>
+          <t>avramzon</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>sharona</t>
+          <t>amir</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>bachar</t>
+          <t>babikov</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>uriel</t>
+          <t>sharona</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>bali</t>
+          <t>bachar</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>shlomi</t>
+          <t>uriel</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>balykin</t>
+          <t>bali</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>alexey</t>
+          <t>shlomi</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>band</t>
+          <t>balykin</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>gabriel</t>
+          <t>alexey</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>barak</t>
+          <t>band</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>aloni</t>
+          <t>gabriel</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>barber</t>
+          <t>barak</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>eyal</t>
+          <t>aloni</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>barkat</t>
+          <t>barber</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>bian</t>
+          <t>eyal</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>barkolin</t>
+          <t>barkat</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>liron</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>bian</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>becker</t>
+          <t>barkolin</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>josh</t>
+          <t>liron</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ben atar</t>
+          <t>becker</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>orit</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>josh</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ben shlomo</t>
+          <t>ben atar</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>gili</t>
+          <t>orit</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>bernanka</t>
+          <t>ben shlomo</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>sigal</t>
+          <t>gili</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>bibas</t>
+          <t>bernanka</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>osher</t>
+          <t>sigal</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>biton</t>
+          <t>bibas</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>itzik</t>
+          <t>osher</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>blumshtein</t>
+          <t>biton</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>lior</t>
+          <t>itzik</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>bokovza</t>
+          <t>blumshtein</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>yonatan</t>
+          <t>lior</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>braunstein</t>
+          <t>bokovza</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>lior</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>yonatan</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>bruchim</t>
+          <t>braunstein</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>sinay</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>lior</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>bundarker</t>
+          <t>bruchim</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>eitan</t>
+          <t>sinay</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>buskila</t>
+          <t>bundarker</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>omer</t>
+          <t>eitan</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>chernyavsky</t>
+          <t>buskila</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>eduard</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>omer</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>cohen</t>
+          <t>chernyavsky</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>oren</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>eduard</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1118,10 +1155,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>tomer</t>
+          <t>oren</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1131,57 +1169,53 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>moti</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>tomer</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>cohn</t>
+          <t>cohen</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>evgeny</t>
+          <t>moti</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>czitron</t>
+          <t>cohn</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>liron</t>
+          <t>evgeny</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>dachbash</t>
+          <t>czitron</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>tomer</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>liron</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1191,248 +1225,267 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>liora</t>
+          <t>tomer</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>dahan</t>
+          <t>dachbash</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>limor</t>
+          <t>liora</t>
         </is>
       </c>
       <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>dakar</t>
+          <t>dahan</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>dan</t>
+          <t>limor</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>daliot</t>
+          <t>dakar</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>asaf</t>
+          <t>dan</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>daniel</t>
+          <t>daliot</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>hila</t>
+          <t>asaf</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>darhi</t>
+          <t>daniel</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>shay</t>
+          <t>hila</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>daus</t>
+          <t>darhi</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>yarden</t>
+          <t>shay</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>david</t>
+          <t>daus</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>ofir</t>
+          <t>yarden</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>dayan</t>
+          <t>david</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>inbal</t>
+          <t>ofir</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>de levi</t>
+          <t>dayan</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>eli</t>
+          <t>inbal</t>
         </is>
       </c>
       <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>deautsch</t>
+          <t>de levi</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>mili</t>
+          <t>eli</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>debutton</t>
+          <t>deautsch</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>idan</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>mili</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>dishi</t>
+          <t>debutton</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>avraham</t>
+          <t>idan</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>donskoy</t>
+          <t>dishi</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>dmitri</t>
+          <t>avraham</t>
         </is>
       </c>
       <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>dror</t>
+          <t>donskoy</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>shlomi</t>
+          <t>dmitri</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>edlshteyn</t>
+          <t>dror</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>yan</t>
+          <t>shlomi</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>edri</t>
+          <t>edlshteyn</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>eli</t>
+          <t>yan</t>
         </is>
       </c>
       <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>el-abed</t>
+          <t>edri</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>hadeel</t>
+          <t>eli</t>
         </is>
       </c>
       <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>elbaz</t>
+          <t>el-abed</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>shlomi</t>
+          <t>hadeel</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1442,92 +1495,95 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>lior</t>
+          <t>shlomi</t>
         </is>
       </c>
       <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>elbaze</t>
+          <t>elbaz</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>caroline</t>
+          <t>lior</t>
         </is>
       </c>
       <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>elias-yafe</t>
+          <t>elbaze</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>sima</t>
+          <t>caroline</t>
         </is>
       </c>
       <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>elimelech</t>
+          <t>elias-yafe</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>arie</t>
+          <t>sima</t>
         </is>
       </c>
       <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>eliyahu</t>
+          <t>elimelech</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>tamir</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>arie</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>ellyakim</t>
+          <t>eliyahu</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>netta</t>
+          <t>tamir</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>ezra</t>
+          <t>ellyakim</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>tair</t>
+          <t>netta</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1537,40 +1593,39 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>yair</t>
+          <t>tair</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>farhoud</t>
+          <t>ezra</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>zyad</t>
+          <t>yair</t>
         </is>
       </c>
       <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>fisher</t>
+          <t>farhoud</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>lawrence</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>zyad</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1580,170 +1635,179 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>arya</t>
+          <t>lawrence</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>fraij</t>
+          <t>fisher</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>rawnak</t>
+          <t>arya</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>friedrich</t>
+          <t>fraij</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>avraham</t>
+          <t>rawnak</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>froind</t>
+          <t>friedrich</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>tali</t>
+          <t>avraham</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>gamzeletova</t>
+          <t>froind</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>edmond</t>
+          <t>tali</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>gat</t>
+          <t>gamzeletova</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>liat</t>
+          <t>edmond</t>
         </is>
       </c>
       <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>gedassi</t>
+          <t>gat</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>yossi</t>
+          <t>liat</t>
         </is>
       </c>
       <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>geronimus</t>
+          <t>gedassi</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>yuri</t>
+          <t>yossi</t>
         </is>
       </c>
       <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>gitter</t>
+          <t>geronimus</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>hila</t>
+          <t>yuri</t>
         </is>
       </c>
       <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>golan</t>
+          <t>gitter</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>ronit gili</t>
+          <t>hila</t>
         </is>
       </c>
       <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>goldish</t>
+          <t>golan</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>zev</t>
+          <t>ronit gili</t>
         </is>
       </c>
       <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>gonsharovich</t>
+          <t>goldish</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>eldad</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>zev</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>gotfrid</t>
+          <t>gonsharovich</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>maayan</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
+          <t>eldad</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1752,339 +1816,352 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>gur leonzini</t>
+          <t>gotfrid</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>ronen</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>maayan</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>gurevich</t>
+          <t>gur leonzini</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>ala</t>
+          <t>ronen</t>
         </is>
       </c>
       <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t xml:space="preserve">gutman </t>
+          <t>gurevich</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>koby shabby</t>
+          <t>ala</t>
         </is>
       </c>
       <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>habani</t>
+          <t xml:space="preserve">gutman </t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>oriya</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>koby shabby</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>hadad</t>
+          <t>habani</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>hodaya</t>
+          <t>oriya</t>
         </is>
       </c>
       <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>haham</t>
+          <t>hadad</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>ori</t>
+          <t>hodaya</t>
         </is>
       </c>
       <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>haj yahia</t>
+          <t>haham</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>mariam</t>
+          <t>ori</t>
         </is>
       </c>
       <c r="C103" t="inlineStr"/>
+      <c r="D103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>haj -yehia</t>
+          <t>haj yahia</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>amir</t>
+          <t>mariam</t>
         </is>
       </c>
       <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>hajbi</t>
+          <t>haj -yehia</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>lia</t>
+          <t>amir</t>
         </is>
       </c>
       <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>hala</t>
+          <t>hajbi</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>sharon</t>
+          <t>lia</t>
         </is>
       </c>
       <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>halevi</t>
+          <t>hala</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>limor</t>
+          <t>sharon</t>
         </is>
       </c>
       <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>hamoudi</t>
+          <t>halevi</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>amir</t>
+          <t>limor</t>
         </is>
       </c>
       <c r="C108" t="inlineStr"/>
+      <c r="D108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>hanin</t>
+          <t>hamoudi</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>amit</t>
+          <t>amir</t>
         </is>
       </c>
       <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>haster</t>
+          <t>hanin</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>maor</t>
+          <t>amit</t>
         </is>
       </c>
       <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>heletz</t>
+          <t>haster</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>ronen</t>
+          <t>maor</t>
         </is>
       </c>
       <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>hermel</t>
+          <t>heletz</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>ido</t>
+          <t>ronen</t>
         </is>
       </c>
       <c r="C112" t="inlineStr"/>
+      <c r="D112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>hillel</t>
+          <t>hermel</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>nohar</t>
+          <t>ido</t>
         </is>
       </c>
       <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>hlazkov</t>
+          <t>hillel</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>andrii</t>
+          <t>nohar</t>
         </is>
       </c>
       <c r="C114" t="inlineStr"/>
+      <c r="D114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>horesh</t>
+          <t>hlazkov</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>meny</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>andrii</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>hoter</t>
+          <t>horesh</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>avital</t>
+          <t>meny</t>
         </is>
       </c>
       <c r="C116" t="inlineStr"/>
+      <c r="D116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>irmiyahoo</t>
+          <t>hoter</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>liat</t>
+          <t>avital</t>
         </is>
       </c>
       <c r="C117" t="inlineStr"/>
+      <c r="D117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>isakov</t>
+          <t>irmiyahoo</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>moshe</t>
+          <t>liat</t>
         </is>
       </c>
       <c r="C118" t="inlineStr"/>
+      <c r="D118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>israeli</t>
+          <t>isakov</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>bar</t>
+          <t>moshe</t>
         </is>
       </c>
       <c r="C119" t="inlineStr"/>
+      <c r="D119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>itach</t>
+          <t>israeli</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>itzik</t>
+          <t>bar</t>
         </is>
       </c>
       <c r="C120" t="inlineStr"/>
+      <c r="D120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>itzhak</t>
+          <t>itach</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>shiran</t>
+          <t>itzik</t>
         </is>
       </c>
       <c r="C121" t="inlineStr"/>
+      <c r="D121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2094,135 +2171,137 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>golan</t>
+          <t>shiran</t>
         </is>
       </c>
       <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>ivan</t>
+          <t>itzhak</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>avishag</t>
+          <t>golan</t>
         </is>
       </c>
       <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>izkovitch</t>
+          <t>ivan</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>ifat</t>
+          <t>avishag</t>
         </is>
       </c>
       <c r="C124" t="inlineStr"/>
+      <c r="D124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>jabareen</t>
+          <t>izkovitch</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>mohammad</t>
-        </is>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>ifat</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr"/>
+      <c r="D125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>japarov</t>
+          <t>jabareen</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>kiril</t>
+          <t>mohammad</t>
         </is>
       </c>
       <c r="C126" t="inlineStr"/>
+      <c r="D126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>jbara</t>
+          <t>japarov</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>sameer</t>
+          <t>kiril</t>
         </is>
       </c>
       <c r="C127" t="inlineStr"/>
+      <c r="D127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>kahlon</t>
+          <t>jbara</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>yaniv</t>
+          <t>sameer</t>
         </is>
       </c>
       <c r="C128" t="inlineStr"/>
+      <c r="D128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>kasman</t>
+          <t>kahlon</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>peter</t>
-        </is>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>yaniv</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr"/>
+      <c r="D129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>katanov</t>
+          <t>kasman</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>alex</t>
+          <t>peter</t>
         </is>
       </c>
       <c r="C130" t="inlineStr"/>
+      <c r="D130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>katz</t>
+          <t>katanov</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>ilana</t>
+          <t>alex</t>
         </is>
       </c>
       <c r="C131" t="inlineStr"/>
+      <c r="D131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -2232,10 +2311,11 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>mussi</t>
+          <t>ilana</t>
         </is>
       </c>
       <c r="C132" t="inlineStr"/>
+      <c r="D132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -2245,261 +2325,277 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>aviv</t>
+          <t>mussi</t>
         </is>
       </c>
       <c r="C133" t="inlineStr"/>
+      <c r="D133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>katzover</t>
+          <t>katz</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>rachel</t>
+          <t>aviv</t>
         </is>
       </c>
       <c r="C134" t="inlineStr"/>
+      <c r="D134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>katzur</t>
+          <t>katzover</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>hagit</t>
+          <t>rachel</t>
         </is>
       </c>
       <c r="C135" t="inlineStr"/>
+      <c r="D135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>keinan</t>
+          <t>katzur</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>yair</t>
+          <t>hagit</t>
         </is>
       </c>
       <c r="C136" t="inlineStr"/>
+      <c r="D136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>kerner</t>
+          <t>keinan</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>amit</t>
+          <t>yair</t>
         </is>
       </c>
       <c r="C137" t="inlineStr"/>
+      <c r="D137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>khalhni</t>
+          <t>kerner</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>lital</t>
+          <t>amit</t>
         </is>
       </c>
       <c r="C138" t="inlineStr"/>
+      <c r="D138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>kilshtein</t>
+          <t>khalhni</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>daniel</t>
+          <t>lital</t>
         </is>
       </c>
       <c r="C139" t="inlineStr"/>
+      <c r="D139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>kleiman</t>
+          <t>kilshtein</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>yarden</t>
+          <t>daniel</t>
         </is>
       </c>
       <c r="C140" t="inlineStr"/>
+      <c r="D140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>klein</t>
+          <t>kleiman</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>yacov</t>
-        </is>
-      </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>yarden</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr"/>
+      <c r="D141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>klipach</t>
+          <t>klein</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>gennadii</t>
+          <t>yacov</t>
         </is>
       </c>
       <c r="C142" t="inlineStr"/>
+      <c r="D142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>kodus</t>
+          <t>klipach</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>dimitry</t>
+          <t>gennadii</t>
         </is>
       </c>
       <c r="C143" t="inlineStr"/>
+      <c r="D143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>kononenko</t>
+          <t>kodus</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>andrii</t>
+          <t>dimitry</t>
         </is>
       </c>
       <c r="C144" t="inlineStr"/>
+      <c r="D144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>kopel</t>
+          <t>kononenko</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>hadar</t>
+          <t>andrii</t>
         </is>
       </c>
       <c r="C145" t="inlineStr"/>
+      <c r="D145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>kremer</t>
+          <t>kopel</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>yaniv</t>
+          <t>hadar</t>
         </is>
       </c>
       <c r="C146" t="inlineStr"/>
+      <c r="D146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>kreplik</t>
+          <t>kremer</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>peter</t>
+          <t>yaniv</t>
         </is>
       </c>
       <c r="C147" t="inlineStr"/>
+      <c r="D147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>krochro</t>
+          <t>kreplik</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>arik</t>
+          <t>peter</t>
         </is>
       </c>
       <c r="C148" t="inlineStr"/>
+      <c r="D148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>kurtzband</t>
+          <t>krochro</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>moti</t>
+          <t>arik</t>
         </is>
       </c>
       <c r="C149" t="inlineStr"/>
+      <c r="D149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>lavi</t>
+          <t>kurtzband</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>haim</t>
+          <t>moti</t>
         </is>
       </c>
       <c r="C150" t="inlineStr"/>
+      <c r="D150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>lederman</t>
+          <t>lavi</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>emanuel</t>
+          <t>haim</t>
         </is>
       </c>
       <c r="C151" t="inlineStr"/>
+      <c r="D151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>levi</t>
+          <t>lederman</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>liran</t>
+          <t>emanuel</t>
         </is>
       </c>
       <c r="C152" t="inlineStr"/>
+      <c r="D152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -2509,10 +2605,11 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>inbal</t>
+          <t>liran</t>
         </is>
       </c>
       <c r="C153" t="inlineStr"/>
+      <c r="D153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -2522,10 +2619,11 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>liraz</t>
+          <t>inbal</t>
         </is>
       </c>
       <c r="C154" t="inlineStr"/>
+      <c r="D154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -2535,10 +2633,11 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>paz</t>
+          <t>liraz</t>
         </is>
       </c>
       <c r="C155" t="inlineStr"/>
+      <c r="D155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -2548,10 +2647,11 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>mazal</t>
+          <t>paz</t>
         </is>
       </c>
       <c r="C156" t="inlineStr"/>
+      <c r="D156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -2561,10 +2661,11 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>asaf</t>
+          <t>mazal</t>
         </is>
       </c>
       <c r="C157" t="inlineStr"/>
+      <c r="D157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -2574,235 +2675,249 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>idan</t>
+          <t>asaf</t>
         </is>
       </c>
       <c r="C158" t="inlineStr"/>
+      <c r="D158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>levy</t>
+          <t>levi</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>sharon</t>
+          <t>idan</t>
         </is>
       </c>
       <c r="C159" t="inlineStr"/>
+      <c r="D159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>liberman</t>
+          <t>levy</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>mark</t>
+          <t>sharon</t>
         </is>
       </c>
       <c r="C160" t="inlineStr"/>
+      <c r="D160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>lieber</t>
+          <t>liberman</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>nadav</t>
+          <t>mark</t>
         </is>
       </c>
       <c r="C161" t="inlineStr"/>
+      <c r="D161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>lieberman</t>
+          <t>lieber</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>vera</t>
+          <t>nadav</t>
         </is>
       </c>
       <c r="C162" t="inlineStr"/>
+      <c r="D162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>lugasi</t>
+          <t>lieberman</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>yael</t>
+          <t>vera</t>
         </is>
       </c>
       <c r="C163" t="inlineStr"/>
+      <c r="D163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>machpud</t>
+          <t>lugasi</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>hila</t>
+          <t>yael</t>
         </is>
       </c>
       <c r="C164" t="inlineStr"/>
+      <c r="D164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>mahluf</t>
+          <t>machpud</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>asaf</t>
+          <t>hila</t>
         </is>
       </c>
       <c r="C165" t="inlineStr"/>
+      <c r="D165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>mahrat</t>
+          <t>mahluf</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>or</t>
+          <t>asaf</t>
         </is>
       </c>
       <c r="C166" t="inlineStr"/>
+      <c r="D166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>malihi</t>
+          <t>mahrat</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>erez</t>
+          <t>or</t>
         </is>
       </c>
       <c r="C167" t="inlineStr"/>
+      <c r="D167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>maman</t>
+          <t>malihi</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>jonas</t>
-        </is>
-      </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>erez</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr"/>
+      <c r="D168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>man</t>
+          <t>maman</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>federico</t>
+          <t>jonas</t>
         </is>
       </c>
       <c r="C169" t="inlineStr"/>
+      <c r="D169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>manoah</t>
+          <t>man</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>alon</t>
+          <t>federico</t>
         </is>
       </c>
       <c r="C170" t="inlineStr"/>
+      <c r="D170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>manzur</t>
+          <t>manoah</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>moran</t>
+          <t>alon</t>
         </is>
       </c>
       <c r="C171" t="inlineStr"/>
+      <c r="D171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>marachev</t>
+          <t>manzur</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>egor</t>
+          <t>moran</t>
         </is>
       </c>
       <c r="C172" t="inlineStr"/>
+      <c r="D172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>marek</t>
+          <t>marachev</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>daniel</t>
+          <t>egor</t>
         </is>
       </c>
       <c r="C173" t="inlineStr"/>
+      <c r="D173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>maruali</t>
+          <t>marek</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>avi</t>
+          <t>daniel</t>
         </is>
       </c>
       <c r="C174" t="inlineStr"/>
+      <c r="D174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>meir</t>
+          <t>maruali</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>chen</t>
+          <t>avi</t>
         </is>
       </c>
       <c r="C175" t="inlineStr"/>
+      <c r="D175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -2812,105 +2927,109 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>shiran</t>
+          <t>chen</t>
         </is>
       </c>
       <c r="C176" t="inlineStr"/>
+      <c r="D176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>meiri</t>
+          <t>meir</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>shai</t>
+          <t>shiran</t>
         </is>
       </c>
       <c r="C177" t="inlineStr"/>
+      <c r="D177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>melion</t>
+          <t>meiri</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>rafi</t>
+          <t>shai</t>
         </is>
       </c>
       <c r="C178" t="inlineStr"/>
+      <c r="D178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>menashe</t>
+          <t>melion</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>laurie-michelle</t>
-        </is>
-      </c>
-      <c r="C179" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>rafi</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr"/>
+      <c r="D179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>milara</t>
+          <t>menashe</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>yossi</t>
+          <t>laurie-michelle</t>
         </is>
       </c>
       <c r="C180" t="inlineStr"/>
+      <c r="D180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>mishani</t>
+          <t>milara</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>yael</t>
+          <t>yossi</t>
         </is>
       </c>
       <c r="C181" t="inlineStr"/>
+      <c r="D181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>mitlansky</t>
+          <t>mishani</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>rina</t>
+          <t>yael</t>
         </is>
       </c>
       <c r="C182" t="inlineStr"/>
+      <c r="D182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>mizrahi</t>
+          <t>mitlansky</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>nir</t>
+          <t>rina</t>
         </is>
       </c>
       <c r="C183" t="inlineStr"/>
+      <c r="D183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -2920,105 +3039,109 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>gal</t>
+          <t>nir</t>
         </is>
       </c>
       <c r="C184" t="inlineStr"/>
+      <c r="D184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>mogilevskiy</t>
+          <t>mizrahi</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>andrey</t>
+          <t>gal</t>
         </is>
       </c>
       <c r="C185" t="inlineStr"/>
+      <c r="D185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>moyal</t>
+          <t>mogilevskiy</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>amit</t>
+          <t>andrey</t>
         </is>
       </c>
       <c r="C186" t="inlineStr"/>
+      <c r="D186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>msarwa</t>
+          <t>moyal</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>fatema</t>
+          <t>amit</t>
         </is>
       </c>
       <c r="C187" t="inlineStr"/>
+      <c r="D187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>muhamad</t>
+          <t>msarwa</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>badeer</t>
-        </is>
-      </c>
-      <c r="C188" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>fatema</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr"/>
+      <c r="D188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>nachmani</t>
+          <t>muhamad</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>eli</t>
+          <t>badeer</t>
         </is>
       </c>
       <c r="C189" t="inlineStr"/>
+      <c r="D189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>nagar</t>
+          <t>nachmani</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>yarit</t>
+          <t>eli</t>
         </is>
       </c>
       <c r="C190" t="inlineStr"/>
+      <c r="D190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>nahari</t>
+          <t>nagar</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>or</t>
+          <t>yarit</t>
         </is>
       </c>
       <c r="C191" t="inlineStr"/>
+      <c r="D191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -3028,919 +3151,981 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>ori</t>
+          <t>or</t>
         </is>
       </c>
       <c r="C192" t="inlineStr"/>
+      <c r="D192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>nahum</t>
+          <t>nahari</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>suzan</t>
+          <t>ori</t>
         </is>
       </c>
       <c r="C193" t="inlineStr"/>
+      <c r="D193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>najeeb</t>
+          <t>nahum</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>kheir</t>
+          <t>suzan</t>
         </is>
       </c>
       <c r="C194" t="inlineStr"/>
+      <c r="D194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>nechushtan</t>
+          <t>najeeb</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>liat</t>
+          <t>kheir</t>
         </is>
       </c>
       <c r="C195" t="inlineStr"/>
+      <c r="D195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>nevo</t>
+          <t>nechushtan</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>tomer</t>
+          <t>liat</t>
         </is>
       </c>
       <c r="C196" t="inlineStr"/>
+      <c r="D196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>nisani</t>
+          <t>nevo</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>liora</t>
+          <t>tomer</t>
         </is>
       </c>
       <c r="C197" t="inlineStr"/>
+      <c r="D197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>nissim</t>
+          <t>nisani</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>hoshen</t>
+          <t>liora</t>
         </is>
       </c>
       <c r="C198" t="inlineStr"/>
+      <c r="D198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>nogard</t>
+          <t>nissim</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>barak</t>
+          <t>hoshen</t>
         </is>
       </c>
       <c r="C199" t="inlineStr"/>
+      <c r="D199" t="inlineStr"/>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>nouriani</t>
+          <t>nogard</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>elior</t>
+          <t>barak</t>
         </is>
       </c>
       <c r="C200" t="inlineStr"/>
+      <c r="D200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>ohana</t>
+          <t>nouriani</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>elisheva</t>
+          <t>elior</t>
         </is>
       </c>
       <c r="C201" t="inlineStr"/>
+      <c r="D201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>ohayon</t>
+          <t>ohana</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>oz</t>
+          <t>elisheva</t>
         </is>
       </c>
       <c r="C202" t="inlineStr"/>
+      <c r="D202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>opochinsky</t>
+          <t>ohayon</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>yair yaacov</t>
+          <t>oz</t>
         </is>
       </c>
       <c r="C203" t="inlineStr"/>
+      <c r="D203" t="inlineStr"/>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>ovadya</t>
+          <t>opochinsky</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>maayan</t>
+          <t>yair yaacov</t>
         </is>
       </c>
       <c r="C204" t="inlineStr"/>
+      <c r="D204" t="inlineStr"/>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>oz -ari</t>
+          <t>ovadya</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>uri</t>
+          <t>maayan</t>
         </is>
       </c>
       <c r="C205" t="inlineStr"/>
+      <c r="D205" t="inlineStr"/>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>paltiel</t>
+          <t>oz -ari</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>barak</t>
+          <t>uri</t>
         </is>
       </c>
       <c r="C206" t="inlineStr"/>
+      <c r="D206" t="inlineStr"/>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>papashvili</t>
+          <t>paltiel</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>manana</t>
+          <t>barak</t>
         </is>
       </c>
       <c r="C207" t="inlineStr"/>
+      <c r="D207" t="inlineStr"/>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>pashutin</t>
+          <t>papashvili</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>yakir victor</t>
+          <t>manana</t>
         </is>
       </c>
       <c r="C208" t="inlineStr"/>
+      <c r="D208" t="inlineStr"/>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>peled</t>
+          <t>pashutin</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>orly</t>
+          <t>yakir victor</t>
         </is>
       </c>
       <c r="C209" t="inlineStr"/>
+      <c r="D209" t="inlineStr"/>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>peretz</t>
+          <t>peled</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>elinor</t>
+          <t>orly</t>
         </is>
       </c>
       <c r="C210" t="inlineStr"/>
+      <c r="D210" t="inlineStr"/>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>perry</t>
+          <t>peretz</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>efrat</t>
+          <t>elinor</t>
         </is>
       </c>
       <c r="C211" t="inlineStr"/>
+      <c r="D211" t="inlineStr"/>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>petrosian</t>
+          <t>perry</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>asia</t>
+          <t>efrat</t>
         </is>
       </c>
       <c r="C212" t="inlineStr"/>
+      <c r="D212" t="inlineStr"/>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>pilipchuk</t>
+          <t>petrosian</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>ivan</t>
+          <t>asia</t>
         </is>
       </c>
       <c r="C213" t="inlineStr"/>
+      <c r="D213" t="inlineStr"/>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>poraz wachtel</t>
+          <t>pilipchuk</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>dori</t>
+          <t>ivan</t>
         </is>
       </c>
       <c r="C214" t="inlineStr"/>
+      <c r="D214" t="inlineStr"/>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>qasim</t>
+          <t>poraz wachtel</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>nadin</t>
+          <t>dori</t>
         </is>
       </c>
       <c r="C215" t="inlineStr"/>
+      <c r="D215" t="inlineStr"/>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>ratzon</t>
+          <t>qasim</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>liel</t>
+          <t>nadin</t>
         </is>
       </c>
       <c r="C216" t="inlineStr"/>
+      <c r="D216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>ravid</t>
+          <t>ratzon</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>maayan</t>
+          <t>liel</t>
         </is>
       </c>
       <c r="C217" t="inlineStr"/>
+      <c r="D217" t="inlineStr"/>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>raviv</t>
+          <t>ravid</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>omer</t>
+          <t>maayan</t>
         </is>
       </c>
       <c r="C218" t="inlineStr"/>
+      <c r="D218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>riza</t>
+          <t>raviv</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>raviv</t>
+          <t>omer</t>
         </is>
       </c>
       <c r="C219" t="inlineStr"/>
+      <c r="D219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>roffe</t>
+          <t>riza</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>eyal</t>
+          <t>raviv</t>
         </is>
       </c>
       <c r="C220" t="inlineStr"/>
+      <c r="D220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>roitberg</t>
+          <t>roffe</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>alfred</t>
+          <t>eyal</t>
         </is>
       </c>
       <c r="C221" t="inlineStr"/>
+      <c r="D221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>romano</t>
+          <t>roitberg</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>chen</t>
+          <t>alfred</t>
         </is>
       </c>
       <c r="C222" t="inlineStr"/>
+      <c r="D222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>rotshild</t>
+          <t>romano</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>hagai</t>
+          <t>chen</t>
         </is>
       </c>
       <c r="C223" t="inlineStr"/>
+      <c r="D223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>rozen</t>
+          <t>rotshild</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>kobi</t>
+          <t>hagai</t>
         </is>
       </c>
       <c r="C224" t="inlineStr"/>
+      <c r="D224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>rubin</t>
+          <t>rozen</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>almog</t>
+          <t>kobi</t>
         </is>
       </c>
       <c r="C225" t="inlineStr"/>
+      <c r="D225" t="inlineStr"/>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>saad</t>
+          <t>rubin</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>yehiel</t>
+          <t>almog</t>
         </is>
       </c>
       <c r="C226" t="inlineStr"/>
+      <c r="D226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>sabach</t>
+          <t>saad</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>merav</t>
+          <t>yehiel</t>
         </is>
       </c>
       <c r="C227" t="inlineStr"/>
+      <c r="D227" t="inlineStr"/>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>sabi</t>
+          <t>sabach</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>liat</t>
+          <t>merav</t>
         </is>
       </c>
       <c r="C228" t="inlineStr"/>
+      <c r="D228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>sagron</t>
+          <t>sabi</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>snir</t>
+          <t>liat</t>
         </is>
       </c>
       <c r="C229" t="inlineStr"/>
+      <c r="D229" t="inlineStr"/>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>sahar shaba</t>
+          <t>sagron</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>einat</t>
+          <t>snir</t>
         </is>
       </c>
       <c r="C230" t="inlineStr"/>
+      <c r="D230" t="inlineStr"/>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>sany</t>
+          <t>sahar shaba</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>avi</t>
+          <t>einat</t>
         </is>
       </c>
       <c r="C231" t="inlineStr"/>
+      <c r="D231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>savat</t>
+          <t>sany</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>yakov</t>
+          <t>avi</t>
         </is>
       </c>
       <c r="C232" t="inlineStr"/>
+      <c r="D232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>savitzky</t>
+          <t>savat</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>dikla</t>
+          <t>yakov</t>
         </is>
       </c>
       <c r="C233" t="inlineStr"/>
+      <c r="D233" t="inlineStr"/>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>sayuk</t>
+          <t>savitzky</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>benny</t>
+          <t>dikla</t>
         </is>
       </c>
       <c r="C234" t="inlineStr"/>
+      <c r="D234" t="inlineStr"/>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>segal</t>
+          <t>sayuk</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>oded</t>
+          <t>benny</t>
         </is>
       </c>
       <c r="C235" t="inlineStr"/>
+      <c r="D235" t="inlineStr"/>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>segev</t>
+          <t>segal</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>shaked</t>
+          <t>oded</t>
         </is>
       </c>
       <c r="C236" t="inlineStr"/>
+      <c r="D236" t="inlineStr"/>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>shabi</t>
+          <t>segev</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>shai</t>
+          <t>shaked</t>
         </is>
       </c>
       <c r="C237" t="inlineStr"/>
+      <c r="D237" t="inlineStr"/>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>shaida</t>
+          <t>shabi</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>sagi</t>
+          <t>shai</t>
         </is>
       </c>
       <c r="C238" t="inlineStr"/>
+      <c r="D238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>shaked</t>
+          <t>shaida</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>ofra</t>
+          <t>sagi</t>
         </is>
       </c>
       <c r="C239" t="inlineStr"/>
+      <c r="D239" t="inlineStr"/>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>shalev</t>
+          <t>shaked</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>gal</t>
+          <t>ofra</t>
         </is>
       </c>
       <c r="C240" t="inlineStr"/>
+      <c r="D240" t="inlineStr"/>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>shalil</t>
+          <t>shalev</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>zehava</t>
+          <t>gal</t>
         </is>
       </c>
       <c r="C241" t="inlineStr"/>
+      <c r="D241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>shalom</t>
+          <t>shalil</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>nuphar</t>
+          <t>zehava</t>
         </is>
       </c>
       <c r="C242" t="inlineStr"/>
+      <c r="D242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>shapira</t>
+          <t>shalom</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>shai</t>
-        </is>
-      </c>
-      <c r="C243" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>nuphar</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr"/>
+      <c r="D243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>sharem</t>
+          <t>shapira</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>moshe</t>
+          <t>shai</t>
         </is>
       </c>
       <c r="C244" t="inlineStr"/>
+      <c r="D244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>shasha</t>
+          <t>sharem</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>rotem</t>
+          <t>moshe</t>
         </is>
       </c>
       <c r="C245" t="inlineStr"/>
+      <c r="D245" t="inlineStr"/>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>shaul</t>
+          <t>shasha</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>adi</t>
+          <t>rotem</t>
         </is>
       </c>
       <c r="C246" t="inlineStr"/>
+      <c r="D246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>shayo</t>
+          <t>shaul</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>yaacov gilad</t>
+          <t>adi</t>
         </is>
       </c>
       <c r="C247" t="inlineStr"/>
+      <c r="D247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>shefi</t>
+          <t>shayo</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>ariel</t>
+          <t>yaacov gilad</t>
         </is>
       </c>
       <c r="C248" t="inlineStr"/>
+      <c r="D248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>sheinfeld</t>
+          <t>shefi</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>asaf</t>
+          <t>ariel</t>
         </is>
       </c>
       <c r="C249" t="inlineStr"/>
+      <c r="D249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>shimon</t>
+          <t>sheinfeld</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>aviad</t>
+          <t>asaf</t>
         </is>
       </c>
       <c r="C250" t="inlineStr"/>
+      <c r="D250" t="inlineStr"/>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>shirvi</t>
+          <t>shimon</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>shiran</t>
+          <t>aviad</t>
         </is>
       </c>
       <c r="C251" t="inlineStr"/>
+      <c r="D251" t="inlineStr"/>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>shkalim</t>
+          <t>shirvi</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>inon</t>
+          <t>shiran</t>
         </is>
       </c>
       <c r="C252" t="inlineStr"/>
+      <c r="D252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>shmartov</t>
+          <t>shkalim</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>nastya</t>
-        </is>
-      </c>
-      <c r="C253" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>inon</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr"/>
+      <c r="D253" t="inlineStr"/>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>shmueli</t>
+          <t>shmartov</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>matanel</t>
+          <t>nastya</t>
         </is>
       </c>
       <c r="C254" t="inlineStr"/>
+      <c r="D254" t="inlineStr"/>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>shtainberg</t>
+          <t>shmueli</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>aita</t>
+          <t>matanel</t>
         </is>
       </c>
       <c r="C255" t="inlineStr"/>
+      <c r="D255" t="inlineStr"/>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>shuali</t>
+          <t>shtainberg</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>yair</t>
+          <t>aita</t>
         </is>
       </c>
       <c r="C256" t="inlineStr"/>
+      <c r="D256" t="inlineStr"/>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>shugalei</t>
+          <t>shuali</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>ivan</t>
+          <t>yair</t>
         </is>
       </c>
       <c r="C257" t="inlineStr"/>
+      <c r="D257" t="inlineStr"/>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>shulman</t>
+          <t>shugalei</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>leonid</t>
+          <t>ivan</t>
         </is>
       </c>
       <c r="C258" t="inlineStr"/>
+      <c r="D258" t="inlineStr"/>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>shuster</t>
+          <t>shulman</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>luiza</t>
+          <t>leonid</t>
         </is>
       </c>
       <c r="C259" t="inlineStr"/>
+      <c r="D259" t="inlineStr"/>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>sinenco</t>
+          <t>shuster</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>peter</t>
-        </is>
-      </c>
-      <c r="C260" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>luiza</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr"/>
+      <c r="D260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>sinvani</t>
+          <t>sinenco</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>moran</t>
+          <t>peter</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
+        <is>
+          <t>limor</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -3949,383 +4134,422 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>soffer</t>
+          <t>sinvani</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>dan</t>
-        </is>
-      </c>
-      <c r="C262" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>moran</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr"/>
+      <c r="D262" t="inlineStr"/>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>soler</t>
+          <t>soffer</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>aviv</t>
+          <t>dan</t>
         </is>
       </c>
       <c r="C263" t="inlineStr"/>
+      <c r="D263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>son</t>
+          <t>soler</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>alex</t>
+          <t>aviv</t>
         </is>
       </c>
       <c r="C264" t="inlineStr"/>
+      <c r="D264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>spades</t>
+          <t>son</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>kiro</t>
+          <t>alex</t>
         </is>
       </c>
       <c r="C265" t="inlineStr"/>
+      <c r="D265" t="inlineStr"/>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>sukner</t>
+          <t>spades</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>roman</t>
+          <t>kiro</t>
         </is>
       </c>
       <c r="C266" t="inlineStr"/>
+      <c r="D266" t="inlineStr"/>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>taigfeld</t>
+          <t>sukner</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>clare</t>
+          <t>roman</t>
         </is>
       </c>
       <c r="C267" t="inlineStr"/>
+      <c r="D267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>tal</t>
+          <t>taigfeld</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>lior</t>
+          <t>clare</t>
         </is>
       </c>
       <c r="C268" t="inlineStr"/>
+      <c r="D268" t="inlineStr"/>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>taspa</t>
+          <t>tal</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>netanel</t>
+          <t>lior</t>
         </is>
       </c>
       <c r="C269" t="inlineStr"/>
+      <c r="D269" t="inlineStr"/>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>tevet</t>
+          <t>taspa</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>roni</t>
+          <t>netanel</t>
         </is>
       </c>
       <c r="C270" t="inlineStr"/>
+      <c r="D270" t="inlineStr"/>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>tzadok</t>
+          <t>tevet</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>ben</t>
+          <t>roni</t>
         </is>
       </c>
       <c r="C271" t="inlineStr"/>
+      <c r="D271" t="inlineStr"/>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>tzafar</t>
+          <t>tzadok</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>adir</t>
+          <t>ben</t>
         </is>
       </c>
       <c r="C272" t="inlineStr"/>
+      <c r="D272" t="inlineStr"/>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>tzuberi</t>
+          <t>tzafar</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>almog</t>
+          <t>adir</t>
         </is>
       </c>
       <c r="C273" t="inlineStr"/>
+      <c r="D273" t="inlineStr"/>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>vahaba</t>
+          <t>tzuberi</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>sivan</t>
+          <t>almog</t>
         </is>
       </c>
       <c r="C274" t="inlineStr"/>
+      <c r="D274" t="inlineStr"/>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>vahav</t>
+          <t>vahaba</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>tehila</t>
+          <t>sivan</t>
         </is>
       </c>
       <c r="C275" t="inlineStr"/>
+      <c r="D275" t="inlineStr"/>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>vainberg</t>
+          <t>vahav</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>alexander</t>
+          <t>tehila</t>
         </is>
       </c>
       <c r="C276" t="inlineStr"/>
+      <c r="D276" t="inlineStr"/>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>vaknin</t>
+          <t>vainberg</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>oren</t>
+          <t>alexander</t>
         </is>
       </c>
       <c r="C277" t="inlineStr"/>
+      <c r="D277" t="inlineStr"/>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>valotker</t>
+          <t>vaknin</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>arie</t>
+          <t>oren</t>
         </is>
       </c>
       <c r="C278" t="inlineStr"/>
+      <c r="D278" t="inlineStr"/>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>vaysman</t>
+          <t>valotker</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>dan</t>
+          <t>arie</t>
         </is>
       </c>
       <c r="C279" t="inlineStr"/>
+      <c r="D279" t="inlineStr"/>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>veisas</t>
+          <t>vaysman</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>daniel</t>
+          <t>dan</t>
         </is>
       </c>
       <c r="C280" t="inlineStr"/>
+      <c r="D280" t="inlineStr"/>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>wase</t>
+          <t>veisas</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>roei</t>
+          <t>daniel</t>
         </is>
       </c>
       <c r="C281" t="inlineStr"/>
+      <c r="D281" t="inlineStr"/>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>wiesz</t>
+          <t>wase</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>oren</t>
+          <t>roei</t>
         </is>
       </c>
       <c r="C282" t="inlineStr"/>
+      <c r="D282" t="inlineStr"/>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>yaakovi</t>
+          <t>wiesz</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>shirli</t>
+          <t>oren</t>
         </is>
       </c>
       <c r="C283" t="inlineStr"/>
+      <c r="D283" t="inlineStr"/>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>zangi</t>
+          <t>yaakovi</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>tal</t>
+          <t>shirli</t>
         </is>
       </c>
       <c r="C284" t="inlineStr"/>
+      <c r="D284" t="inlineStr"/>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>zarhi</t>
+          <t>zangi</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>nir</t>
+          <t>tal</t>
         </is>
       </c>
       <c r="C285" t="inlineStr"/>
+      <c r="D285" t="inlineStr"/>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>zaviv</t>
+          <t>zarhi</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>vered</t>
+          <t>nir</t>
         </is>
       </c>
       <c r="C286" t="inlineStr"/>
+      <c r="D286" t="inlineStr"/>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>zbeadt</t>
+          <t>zaviv</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>waseem</t>
+          <t>vered</t>
         </is>
       </c>
       <c r="C287" t="inlineStr"/>
+      <c r="D287" t="inlineStr"/>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>ziskind</t>
+          <t>zbeadt</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>dotan</t>
+          <t>waseem</t>
         </is>
       </c>
       <c r="C288" t="inlineStr"/>
+      <c r="D288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>zriham</t>
+          <t>ziskind</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>revital</t>
+          <t>dotan</t>
         </is>
       </c>
       <c r="C289" t="inlineStr"/>
+      <c r="D289" t="inlineStr"/>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
+          <t>zriham</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>revital</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr"/>
+      <c r="D290" t="inlineStr"/>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
           <t>zriker</t>
         </is>
       </c>
-      <c r="B290" t="inlineStr">
+      <c r="B291" t="inlineStr">
         <is>
           <t>shulamit</t>
         </is>
       </c>
-      <c r="C290" t="inlineStr"/>
+      <c r="C291" t="inlineStr"/>
+      <c r="D291" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add new button , fix view of table & buttons V1 Test
</commit_message>
<xml_diff>
--- a/uploads/updated_gift_list.xlsx
+++ b/uploads/updated_gift_list.xlsx
@@ -466,11 +466,7 @@
           <t>verifone</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>יוסי</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -484,16 +480,8 @@
           <t>moataz</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">eldad </t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -506,16 +494,8 @@
           <t>shiran</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ronen</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1257,11 +1237,7 @@
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="D57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1806,7 +1782,11 @@
           <t>eldad</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr"/>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>dror</t>
+        </is>
+      </c>
       <c r="D96" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -4120,16 +4100,8 @@
           <t>peter</t>
         </is>
       </c>
-      <c r="C261" t="inlineStr">
-        <is>
-          <t>limor</t>
-        </is>
-      </c>
-      <c r="D261" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C261" t="inlineStr"/>
+      <c r="D261" t="inlineStr"/>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">

</xml_diff>

<commit_message>
new ajusments colors , tables , font V5 try to fix mobile viewV17B
</commit_message>
<xml_diff>
--- a/uploads/updated_gift_list.xlsx
+++ b/uploads/updated_gift_list.xlsx
@@ -466,8 +466,16 @@
           <t>verifone</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>david</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -481,7 +489,11 @@
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -495,7 +507,11 @@
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -509,7 +525,11 @@
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1754,8 +1774,16 @@
           <t>ronit gili</t>
         </is>
       </c>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>gil</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1782,16 +1810,8 @@
           <t>eldad</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>dror</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">

</xml_diff>

<commit_message>
aftre fix phone view , after upload saved excel clear NO at Taken By
</commit_message>
<xml_diff>
--- a/uploads/updated_gift_list.xlsx
+++ b/uploads/updated_gift_list.xlsx
@@ -468,7 +468,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>david</t>
+          <t>רכעקכעקכ</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -506,7 +506,11 @@
           <t>shiran</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>DDDD</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -524,7 +528,11 @@
           <t>zahiya</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>DDDDKJYKJHJ</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -556,8 +564,16 @@
           <t>inbal</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>DVFGHDFVSDGNFGHGH</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1774,16 +1790,8 @@
           <t>ronit gili</t>
         </is>
       </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>gil</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">

</xml_diff>

<commit_message>
add option to undo button -NEW
</commit_message>
<xml_diff>
--- a/uploads/updated_gift_list.xlsx
+++ b/uploads/updated_gift_list.xlsx
@@ -446,12 +446,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Received</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Taken By</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Received</t>
         </is>
       </c>
     </row>
@@ -468,12 +468,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>רכעקכעקכ</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>BOB</t>
         </is>
       </c>
     </row>
@@ -489,11 +489,7 @@
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -506,16 +502,8 @@
           <t>shiran</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>DDDD</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -528,16 +516,8 @@
           <t>zahiya</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>DDDDKJYKJHJ</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -564,16 +544,8 @@
           <t>inbal</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>DVFGHDFVSDGNFGHGH</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -586,7 +558,11 @@
           <t>yakov</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
@@ -628,7 +604,11 @@
           <t>yuval</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
@@ -895,11 +875,7 @@
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="D30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -912,16 +888,8 @@
           <t>alexey</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>YORAM</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1746,7 +1714,11 @@
           <t>liat</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr"/>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
       <c r="D90" t="inlineStr"/>
     </row>
     <row r="91">

</xml_diff>